<commit_message>
Update of the SESMG and the US tool to the new naming convention.
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/plain_scenario.xlsx
+++ b/program_files/urban_district_upscaling/plain_scenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3895DA61-E296-7541-A44E-4153B4AE6BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AD6E57-C9C2-084E-AFAE-158F73A2D64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18840" tabRatio="798" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18540" tabRatio="798" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="32" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="161">
   <si>
     <t>label</t>
   </si>
@@ -188,48 +188,9 @@
     <t>(CU/a)</t>
   </si>
   <si>
-    <t>Turbine Model</t>
-  </si>
-  <si>
-    <t>Hub Height</t>
-  </si>
-  <si>
-    <t>technology database</t>
-  </si>
-  <si>
-    <t>inverter database</t>
-  </si>
-  <si>
-    <t>Modul Model</t>
-  </si>
-  <si>
-    <t>Inverter Model</t>
-  </si>
-  <si>
-    <t>Azimuth</t>
-  </si>
-  <si>
-    <t>Surface Tilt</t>
-  </si>
-  <si>
-    <t>Albedo</t>
-  </si>
-  <si>
-    <t>Altitude</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
     <t>solar heat</t>
   </si>
   <si>
-    <t>Cleanliness</t>
-  </si>
-  <si>
     <t>ETA 0</t>
   </si>
   <si>
@@ -245,21 +206,6 @@
     <t>C2</t>
   </si>
   <si>
-    <t>Peripheral Losses</t>
-  </si>
-  <si>
-    <t>Electric Consumption</t>
-  </si>
-  <si>
-    <t>Temperature Inlet</t>
-  </si>
-  <si>
-    <t>Temperature Difference</t>
-  </si>
-  <si>
-    <t>Conversion Factor</t>
-  </si>
-  <si>
     <t>wind power</t>
   </si>
   <si>
@@ -528,6 +474,54 @@
   </si>
   <si>
     <t>(CU/kW)</t>
+  </si>
+  <si>
+    <t>modul model</t>
+  </si>
+  <si>
+    <t>inverter model</t>
+  </si>
+  <si>
+    <t>albedo</t>
+  </si>
+  <si>
+    <t>altitude</t>
+  </si>
+  <si>
+    <t>azimuth</t>
+  </si>
+  <si>
+    <t>surface tilt</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>turbine model</t>
+  </si>
+  <si>
+    <t>hub height</t>
+  </si>
+  <si>
+    <t>temperature inlet</t>
+  </si>
+  <si>
+    <t>temperature difference</t>
+  </si>
+  <si>
+    <t>conversion factor</t>
+  </si>
+  <si>
+    <t>peripheral losses</t>
+  </si>
+  <si>
+    <t>electric consumption</t>
+  </si>
+  <si>
+    <t>cleanliness</t>
   </si>
 </sst>
 </file>
@@ -821,7 +815,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -943,7 +937,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
@@ -1381,7 +1374,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>15</v>
@@ -1390,57 +1383,57 @@
         <v>26</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="16"/>
       <c r="B3" s="17"/>
-      <c r="C3" s="74"/>
+      <c r="C3" s="73"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1474,19 +1467,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="25" customFormat="1" ht="57">
       <c r="A1" s="29" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F1" s="27" t="s">
         <v>11</v>
@@ -1494,22 +1487,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1946,48 +1939,48 @@
         <v>32</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="L1" s="27" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="N1" s="27" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="O1" s="26" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="P1" s="27" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="3" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>29</v>
@@ -2002,25 +1995,25 @@
         <v>29</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="K2" s="75" t="s">
-        <v>160</v>
-      </c>
-      <c r="L2" s="75" t="s">
-        <v>160</v>
+        <v>131</v>
+      </c>
+      <c r="K2" s="74" t="s">
+        <v>142</v>
+      </c>
+      <c r="L2" s="74" t="s">
+        <v>142</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -2960,33 +2953,33 @@
         <v>37</v>
       </c>
       <c r="J1" s="38" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="K1" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="11" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>34</v>
@@ -3644,14 +3637,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1390354-910C-204E-AADB-46606A5A746C}">
-  <dimension ref="A1:AN50"/>
+  <dimension ref="A1:AL48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B62" sqref="B62"/>
       <selection pane="topRight" activeCell="B62" sqref="B62"/>
       <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
-      <selection pane="bottomRight" activeCell="AM3" sqref="AM3"/>
+      <selection pane="bottomRight" activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" outlineLevelCol="2"/>
@@ -3671,26 +3664,24 @@
     <col min="17" max="17" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="12" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="31" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="39.6640625" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="24" max="24" width="5.1640625" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="7.5" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="27" width="4.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="6.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="5.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="6.1640625" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="31" max="32" width="3.1640625" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="3.33203125" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="36" width="13.33203125" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="16.6640625" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="38" max="38" width="5.1640625" bestFit="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="5.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="4.1640625" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="20" max="20" width="31" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="39.6640625" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="5.1640625" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="7.5" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="25" width="4.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="6.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="5.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="6.1640625" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="29" max="30" width="3.1640625" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="31" max="32" width="3.33203125" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="13.33203125" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="16.6640625" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="5.1640625" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="5.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="4.1640625" bestFit="1" customWidth="1" outlineLevel="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="25" customFormat="1" ht="119">
+    <row r="1" spans="1:38" s="25" customFormat="1" ht="119">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -3722,13 +3713,13 @@
         <v>46</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="L1" s="43" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="M1" s="43" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="N1" s="43" t="s">
         <v>41</v>
@@ -3743,96 +3734,90 @@
         <v>47</v>
       </c>
       <c r="R1" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="S1" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="U1" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="V1" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="W1" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="X1" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y1" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z1" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA1" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB1" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG1" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH1" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI1" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="AJ1" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="AK1" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL1" s="46" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
+      <c r="A2" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="S1" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="W1" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="X1" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y1" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z1" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA1" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB1" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC1" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD1" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE1" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF1" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG1" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH1" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI1" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ1" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK1" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="AL1" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM1" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN1" s="46" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:40">
-      <c r="A2" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="H2" s="47" t="s">
         <v>34</v>
@@ -3844,13 +3829,13 @@
         <v>34</v>
       </c>
       <c r="K2" s="49" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="L2" s="50" t="s">
         <v>48</v>
       </c>
       <c r="M2" s="50" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="N2" s="50" t="s">
         <v>29</v>
@@ -3865,76 +3850,70 @@
         <v>42</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="S2" s="15" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="T2" s="52" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="U2" s="52" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="V2" s="52" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="W2" s="52" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="X2" s="52" t="s">
-        <v>149</v>
+        <v>58</v>
       </c>
       <c r="Y2" s="52" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="Z2" s="52" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="AA2" s="52" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="AB2" s="52" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="AC2" s="52" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="AD2" s="52" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="AE2" s="52" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="AF2" s="52" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="AG2" s="52" t="s">
-        <v>149</v>
+        <v>56</v>
       </c>
       <c r="AH2" s="52" t="s">
-        <v>149</v>
+        <v>56</v>
       </c>
       <c r="AI2" s="52" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="AJ2" s="52" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="AK2" s="52" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="AL2" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM2" s="52" t="s">
-        <v>149</v>
-      </c>
-      <c r="AN2" s="52" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3973,10 +3952,8 @@
       <c r="AJ3" s="5"/>
       <c r="AK3" s="5"/>
       <c r="AL3" s="5"/>
-      <c r="AM3" s="5"/>
-      <c r="AN3" s="5"/>
-    </row>
-    <row r="4" spans="1:40">
+    </row>
+    <row r="4" spans="1:38">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4015,10 +3992,8 @@
       <c r="AJ4" s="6"/>
       <c r="AK4" s="6"/>
       <c r="AL4" s="6"/>
-      <c r="AM4" s="6"/>
-      <c r="AN4" s="6"/>
-    </row>
-    <row r="5" spans="1:40">
+    </row>
+    <row r="5" spans="1:38">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4057,10 +4032,8 @@
       <c r="AJ5" s="5"/>
       <c r="AK5" s="5"/>
       <c r="AL5" s="5"/>
-      <c r="AM5" s="5"/>
-      <c r="AN5" s="5"/>
-    </row>
-    <row r="6" spans="1:40">
+    </row>
+    <row r="6" spans="1:38">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -4099,10 +4072,8 @@
       <c r="AJ6" s="6"/>
       <c r="AK6" s="6"/>
       <c r="AL6" s="6"/>
-      <c r="AM6" s="6"/>
-      <c r="AN6" s="6"/>
-    </row>
-    <row r="7" spans="1:40">
+    </row>
+    <row r="7" spans="1:38">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4141,10 +4112,8 @@
       <c r="AJ7" s="5"/>
       <c r="AK7" s="5"/>
       <c r="AL7" s="5"/>
-      <c r="AM7" s="5"/>
-      <c r="AN7" s="5"/>
-    </row>
-    <row r="8" spans="1:40">
+    </row>
+    <row r="8" spans="1:38">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -4183,10 +4152,8 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="6"/>
-      <c r="AN8" s="6"/>
-    </row>
-    <row r="9" spans="1:40">
+    </row>
+    <row r="9" spans="1:38">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4225,10 +4192,8 @@
       <c r="AJ9" s="5"/>
       <c r="AK9" s="5"/>
       <c r="AL9" s="5"/>
-      <c r="AM9" s="5"/>
-      <c r="AN9" s="5"/>
-    </row>
-    <row r="10" spans="1:40">
+    </row>
+    <row r="10" spans="1:38">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4267,10 +4232,8 @@
       <c r="AJ10" s="6"/>
       <c r="AK10" s="6"/>
       <c r="AL10" s="6"/>
-      <c r="AM10" s="6"/>
-      <c r="AN10" s="6"/>
-    </row>
-    <row r="11" spans="1:40">
+    </row>
+    <row r="11" spans="1:38">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4309,10 +4272,8 @@
       <c r="AJ11" s="5"/>
       <c r="AK11" s="5"/>
       <c r="AL11" s="5"/>
-      <c r="AM11" s="5"/>
-      <c r="AN11" s="5"/>
-    </row>
-    <row r="12" spans="1:40">
+    </row>
+    <row r="12" spans="1:38">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4351,10 +4312,8 @@
       <c r="AJ12" s="6"/>
       <c r="AK12" s="6"/>
       <c r="AL12" s="6"/>
-      <c r="AM12" s="6"/>
-      <c r="AN12" s="6"/>
-    </row>
-    <row r="13" spans="1:40">
+    </row>
+    <row r="13" spans="1:38">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -4393,10 +4352,8 @@
       <c r="AJ13" s="5"/>
       <c r="AK13" s="5"/>
       <c r="AL13" s="5"/>
-      <c r="AM13" s="5"/>
-      <c r="AN13" s="5"/>
-    </row>
-    <row r="14" spans="1:40">
+    </row>
+    <row r="14" spans="1:38">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -4435,10 +4392,8 @@
       <c r="AJ14" s="6"/>
       <c r="AK14" s="6"/>
       <c r="AL14" s="6"/>
-      <c r="AM14" s="6"/>
-      <c r="AN14" s="6"/>
-    </row>
-    <row r="15" spans="1:40">
+    </row>
+    <row r="15" spans="1:38">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4477,10 +4432,8 @@
       <c r="AJ15" s="5"/>
       <c r="AK15" s="5"/>
       <c r="AL15" s="5"/>
-      <c r="AM15" s="5"/>
-      <c r="AN15" s="5"/>
-    </row>
-    <row r="16" spans="1:40">
+    </row>
+    <row r="16" spans="1:38">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -4519,10 +4472,8 @@
       <c r="AJ16" s="6"/>
       <c r="AK16" s="6"/>
       <c r="AL16" s="6"/>
-      <c r="AM16" s="6"/>
-      <c r="AN16" s="6"/>
-    </row>
-    <row r="17" spans="1:40">
+    </row>
+    <row r="17" spans="1:38">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4561,10 +4512,8 @@
       <c r="AJ17" s="5"/>
       <c r="AK17" s="5"/>
       <c r="AL17" s="5"/>
-      <c r="AM17" s="5"/>
-      <c r="AN17" s="5"/>
-    </row>
-    <row r="18" spans="1:40">
+    </row>
+    <row r="18" spans="1:38">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4603,10 +4552,8 @@
       <c r="AJ18" s="6"/>
       <c r="AK18" s="6"/>
       <c r="AL18" s="6"/>
-      <c r="AM18" s="6"/>
-      <c r="AN18" s="6"/>
-    </row>
-    <row r="19" spans="1:40">
+    </row>
+    <row r="19" spans="1:38">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4645,10 +4592,8 @@
       <c r="AJ19" s="5"/>
       <c r="AK19" s="5"/>
       <c r="AL19" s="5"/>
-      <c r="AM19" s="5"/>
-      <c r="AN19" s="5"/>
-    </row>
-    <row r="20" spans="1:40">
+    </row>
+    <row r="20" spans="1:38">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -4687,10 +4632,8 @@
       <c r="AJ20" s="6"/>
       <c r="AK20" s="6"/>
       <c r="AL20" s="6"/>
-      <c r="AM20" s="6"/>
-      <c r="AN20" s="6"/>
-    </row>
-    <row r="21" spans="1:40">
+    </row>
+    <row r="21" spans="1:38">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -4729,10 +4672,8 @@
       <c r="AJ21" s="5"/>
       <c r="AK21" s="5"/>
       <c r="AL21" s="5"/>
-      <c r="AM21" s="5"/>
-      <c r="AN21" s="5"/>
-    </row>
-    <row r="22" spans="1:40">
+    </row>
+    <row r="22" spans="1:38">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -4771,10 +4712,8 @@
       <c r="AJ22" s="6"/>
       <c r="AK22" s="6"/>
       <c r="AL22" s="6"/>
-      <c r="AM22" s="6"/>
-      <c r="AN22" s="6"/>
-    </row>
-    <row r="23" spans="1:40">
+    </row>
+    <row r="23" spans="1:38">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -4813,10 +4752,8 @@
       <c r="AJ23" s="5"/>
       <c r="AK23" s="5"/>
       <c r="AL23" s="5"/>
-      <c r="AM23" s="5"/>
-      <c r="AN23" s="5"/>
-    </row>
-    <row r="24" spans="1:40">
+    </row>
+    <row r="24" spans="1:38">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -4855,10 +4792,8 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
-      <c r="AM24" s="6"/>
-      <c r="AN24" s="6"/>
-    </row>
-    <row r="25" spans="1:40">
+    </row>
+    <row r="25" spans="1:38">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -4897,10 +4832,8 @@
       <c r="AJ25" s="5"/>
       <c r="AK25" s="5"/>
       <c r="AL25" s="5"/>
-      <c r="AM25" s="5"/>
-      <c r="AN25" s="5"/>
-    </row>
-    <row r="26" spans="1:40">
+    </row>
+    <row r="26" spans="1:38">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -4939,10 +4872,8 @@
       <c r="AJ26" s="6"/>
       <c r="AK26" s="6"/>
       <c r="AL26" s="6"/>
-      <c r="AM26" s="6"/>
-      <c r="AN26" s="6"/>
-    </row>
-    <row r="27" spans="1:40">
+    </row>
+    <row r="27" spans="1:38">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -4981,10 +4912,8 @@
       <c r="AJ27" s="5"/>
       <c r="AK27" s="5"/>
       <c r="AL27" s="5"/>
-      <c r="AM27" s="5"/>
-      <c r="AN27" s="5"/>
-    </row>
-    <row r="28" spans="1:40">
+    </row>
+    <row r="28" spans="1:38">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -5023,10 +4952,8 @@
       <c r="AJ28" s="6"/>
       <c r="AK28" s="6"/>
       <c r="AL28" s="6"/>
-      <c r="AM28" s="6"/>
-      <c r="AN28" s="6"/>
-    </row>
-    <row r="29" spans="1:40">
+    </row>
+    <row r="29" spans="1:38">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -5065,10 +4992,8 @@
       <c r="AJ29" s="5"/>
       <c r="AK29" s="5"/>
       <c r="AL29" s="5"/>
-      <c r="AM29" s="5"/>
-      <c r="AN29" s="5"/>
-    </row>
-    <row r="30" spans="1:40">
+    </row>
+    <row r="30" spans="1:38">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -5107,10 +5032,8 @@
       <c r="AJ30" s="6"/>
       <c r="AK30" s="6"/>
       <c r="AL30" s="6"/>
-      <c r="AM30" s="6"/>
-      <c r="AN30" s="6"/>
-    </row>
-    <row r="31" spans="1:40">
+    </row>
+    <row r="31" spans="1:38">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -5149,10 +5072,8 @@
       <c r="AJ31" s="5"/>
       <c r="AK31" s="5"/>
       <c r="AL31" s="5"/>
-      <c r="AM31" s="5"/>
-      <c r="AN31" s="5"/>
-    </row>
-    <row r="32" spans="1:40">
+    </row>
+    <row r="32" spans="1:38">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -5191,10 +5112,8 @@
       <c r="AJ32" s="6"/>
       <c r="AK32" s="6"/>
       <c r="AL32" s="6"/>
-      <c r="AM32" s="6"/>
-      <c r="AN32" s="6"/>
-    </row>
-    <row r="33" spans="1:40">
+    </row>
+    <row r="33" spans="1:38">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -5233,10 +5152,8 @@
       <c r="AJ33" s="5"/>
       <c r="AK33" s="5"/>
       <c r="AL33" s="5"/>
-      <c r="AM33" s="5"/>
-      <c r="AN33" s="5"/>
-    </row>
-    <row r="34" spans="1:40">
+    </row>
+    <row r="34" spans="1:38">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -5275,10 +5192,8 @@
       <c r="AJ34" s="6"/>
       <c r="AK34" s="6"/>
       <c r="AL34" s="6"/>
-      <c r="AM34" s="6"/>
-      <c r="AN34" s="6"/>
-    </row>
-    <row r="35" spans="1:40">
+    </row>
+    <row r="35" spans="1:38">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -5317,10 +5232,8 @@
       <c r="AJ35" s="5"/>
       <c r="AK35" s="5"/>
       <c r="AL35" s="5"/>
-      <c r="AM35" s="5"/>
-      <c r="AN35" s="5"/>
-    </row>
-    <row r="36" spans="1:40">
+    </row>
+    <row r="36" spans="1:38">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -5359,10 +5272,8 @@
       <c r="AJ36" s="6"/>
       <c r="AK36" s="6"/>
       <c r="AL36" s="6"/>
-      <c r="AM36" s="6"/>
-      <c r="AN36" s="6"/>
-    </row>
-    <row r="37" spans="1:40">
+    </row>
+    <row r="37" spans="1:38">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -5401,10 +5312,8 @@
       <c r="AJ37" s="5"/>
       <c r="AK37" s="5"/>
       <c r="AL37" s="5"/>
-      <c r="AM37" s="5"/>
-      <c r="AN37" s="5"/>
-    </row>
-    <row r="38" spans="1:40">
+    </row>
+    <row r="38" spans="1:38">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -5443,10 +5352,8 @@
       <c r="AJ38" s="6"/>
       <c r="AK38" s="6"/>
       <c r="AL38" s="6"/>
-      <c r="AM38" s="6"/>
-      <c r="AN38" s="6"/>
-    </row>
-    <row r="39" spans="1:40">
+    </row>
+    <row r="39" spans="1:38">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -5485,10 +5392,8 @@
       <c r="AJ39" s="5"/>
       <c r="AK39" s="5"/>
       <c r="AL39" s="5"/>
-      <c r="AM39" s="5"/>
-      <c r="AN39" s="5"/>
-    </row>
-    <row r="40" spans="1:40">
+    </row>
+    <row r="40" spans="1:38">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -5527,10 +5432,8 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
-      <c r="AM40" s="6"/>
-      <c r="AN40" s="6"/>
-    </row>
-    <row r="41" spans="1:40">
+    </row>
+    <row r="41" spans="1:38">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -5569,10 +5472,8 @@
       <c r="AJ41" s="5"/>
       <c r="AK41" s="5"/>
       <c r="AL41" s="5"/>
-      <c r="AM41" s="5"/>
-      <c r="AN41" s="5"/>
-    </row>
-    <row r="42" spans="1:40">
+    </row>
+    <row r="42" spans="1:38">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -5611,10 +5512,8 @@
       <c r="AJ42" s="6"/>
       <c r="AK42" s="6"/>
       <c r="AL42" s="6"/>
-      <c r="AM42" s="6"/>
-      <c r="AN42" s="6"/>
-    </row>
-    <row r="43" spans="1:40">
+    </row>
+    <row r="43" spans="1:38">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -5653,10 +5552,8 @@
       <c r="AJ43" s="5"/>
       <c r="AK43" s="5"/>
       <c r="AL43" s="5"/>
-      <c r="AM43" s="5"/>
-      <c r="AN43" s="5"/>
-    </row>
-    <row r="44" spans="1:40">
+    </row>
+    <row r="44" spans="1:38">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -5695,10 +5592,8 @@
       <c r="AJ44" s="6"/>
       <c r="AK44" s="6"/>
       <c r="AL44" s="6"/>
-      <c r="AM44" s="6"/>
-      <c r="AN44" s="6"/>
-    </row>
-    <row r="45" spans="1:40">
+    </row>
+    <row r="45" spans="1:38">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -5737,10 +5632,8 @@
       <c r="AJ45" s="5"/>
       <c r="AK45" s="5"/>
       <c r="AL45" s="5"/>
-      <c r="AM45" s="5"/>
-      <c r="AN45" s="5"/>
-    </row>
-    <row r="46" spans="1:40">
+    </row>
+    <row r="46" spans="1:38">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -5779,10 +5672,8 @@
       <c r="AJ46" s="6"/>
       <c r="AK46" s="6"/>
       <c r="AL46" s="6"/>
-      <c r="AM46" s="6"/>
-      <c r="AN46" s="6"/>
-    </row>
-    <row r="47" spans="1:40">
+    </row>
+    <row r="47" spans="1:38">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -5821,10 +5712,8 @@
       <c r="AJ47" s="5"/>
       <c r="AK47" s="5"/>
       <c r="AL47" s="5"/>
-      <c r="AM47" s="5"/>
-      <c r="AN47" s="5"/>
-    </row>
-    <row r="48" spans="1:40">
+    </row>
+    <row r="48" spans="1:38">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -5863,16 +5752,6 @@
       <c r="AJ48" s="6"/>
       <c r="AK48" s="6"/>
       <c r="AL48" s="6"/>
-      <c r="AM48" s="6"/>
-      <c r="AN48" s="6"/>
-    </row>
-    <row r="49" spans="20:21">
-      <c r="T49" s="59"/>
-      <c r="U49" s="59"/>
-    </row>
-    <row r="50" spans="20:21">
-      <c r="T50" s="59"/>
-      <c r="U50" s="59"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:D48">
@@ -5892,12 +5771,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202E8141-8F15-FF4E-A8C0-0B7CE02C7F8D}">
   <dimension ref="A1:AV46"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B62" sqref="B62"/>
       <selection pane="topRight" activeCell="B62" sqref="B62"/>
       <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
-      <selection pane="bottomRight" activeCell="AW2" sqref="AW2"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" outlineLevelCol="1"/>
@@ -5964,7 +5843,7 @@
       <c r="I1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="60" t="s">
+      <c r="J1" s="59" t="s">
         <v>14</v>
       </c>
       <c r="K1" s="42" t="s">
@@ -5977,13 +5856,13 @@
         <v>46</v>
       </c>
       <c r="N1" s="43" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="O1" s="43" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="P1" s="43" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="Q1" s="43" t="s">
         <v>12</v>
@@ -5992,126 +5871,126 @@
         <v>13</v>
       </c>
       <c r="S1" s="43" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="T1" s="45" t="s">
         <v>43</v>
       </c>
       <c r="U1" s="43" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="V1" s="43" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="W1" s="43" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="X1" s="45" t="s">
         <v>47</v>
       </c>
       <c r="Y1" s="37" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="Z1" s="37" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="AA1" s="37" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="AB1" s="37" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="AC1" s="37" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="AD1" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE1" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF1" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG1" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH1" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI1" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ1" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK1" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL1" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM1" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN1" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO1" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="AP1" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="AQ1" s="60" t="s">
+        <v>114</v>
+      </c>
+      <c r="AR1" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="AS1" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT1" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="AU1" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="AE1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF1" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG1" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH1" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="AI1" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ1" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="AK1" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="AL1" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="AM1" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="AN1" s="61" t="s">
-        <v>129</v>
-      </c>
-      <c r="AO1" s="61" t="s">
-        <v>130</v>
-      </c>
-      <c r="AP1" s="61" t="s">
-        <v>131</v>
-      </c>
-      <c r="AQ1" s="61" t="s">
-        <v>132</v>
-      </c>
-      <c r="AR1" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="AS1" s="61" t="s">
-        <v>134</v>
-      </c>
-      <c r="AT1" s="61" t="s">
-        <v>135</v>
-      </c>
-      <c r="AU1" s="61" t="s">
-        <v>136</v>
-      </c>
-      <c r="AV1" s="61" t="s">
-        <v>137</v>
+      <c r="AV1" s="60" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:48">
       <c r="A2" s="11" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="J2" s="62" t="s">
-        <v>149</v>
+        <v>131</v>
+      </c>
+      <c r="J2" s="61" t="s">
+        <v>131</v>
       </c>
       <c r="K2" s="49" t="s">
         <v>34</v>
@@ -6123,13 +6002,13 @@
         <v>34</v>
       </c>
       <c r="N2" s="50" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="O2" s="50" t="s">
         <v>48</v>
       </c>
       <c r="P2" s="50" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="Q2" s="50" t="s">
         <v>29</v>
@@ -6156,76 +6035,76 @@
         <v>42</v>
       </c>
       <c r="Y2" s="15" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="Z2" s="15" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="AA2" s="15" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="AB2" s="15" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="AC2" s="15" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="AD2" s="15" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="AE2" s="15" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="AF2" s="15" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="AG2" s="15" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="AH2" s="15" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="AI2" s="53" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="AJ2" s="53" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="AK2" s="53" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="AL2" s="53" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="AM2" s="53" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN2" s="63" t="s">
-        <v>149</v>
-      </c>
-      <c r="AO2" s="63" t="s">
-        <v>149</v>
-      </c>
-      <c r="AP2" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN2" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO2" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="AP2" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="AQ2" s="64" t="s">
+      <c r="AQ2" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="AR2" s="63" t="s">
-        <v>149</v>
-      </c>
-      <c r="AS2" s="63" t="s">
-        <v>149</v>
-      </c>
-      <c r="AT2" s="64" t="s">
+      <c r="AR2" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="AS2" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="AT2" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="AU2" s="63" t="s">
-        <v>149</v>
-      </c>
-      <c r="AV2" s="63" t="s">
-        <v>149</v>
+      <c r="AU2" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="AV2" s="62" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:48">
@@ -6268,15 +6147,15 @@
       <c r="AK3" s="5"/>
       <c r="AL3" s="5"/>
       <c r="AM3" s="5"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
-      <c r="AV3" s="65"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+      <c r="AV3" s="64"/>
     </row>
     <row r="4" spans="1:48">
       <c r="A4" s="2"/>
@@ -6318,15 +6197,15 @@
       <c r="AK4" s="6"/>
       <c r="AL4" s="6"/>
       <c r="AM4" s="6"/>
-      <c r="AN4" s="66"/>
-      <c r="AO4" s="66"/>
-      <c r="AP4" s="66"/>
-      <c r="AQ4" s="66"/>
-      <c r="AR4" s="66"/>
-      <c r="AS4" s="66"/>
-      <c r="AT4" s="66"/>
-      <c r="AU4" s="66"/>
-      <c r="AV4" s="66"/>
+      <c r="AN4" s="65"/>
+      <c r="AO4" s="65"/>
+      <c r="AP4" s="65"/>
+      <c r="AQ4" s="65"/>
+      <c r="AR4" s="65"/>
+      <c r="AS4" s="65"/>
+      <c r="AT4" s="65"/>
+      <c r="AU4" s="65"/>
+      <c r="AV4" s="65"/>
     </row>
     <row r="5" spans="1:48">
       <c r="A5" s="1"/>
@@ -6368,15 +6247,15 @@
       <c r="AK5" s="5"/>
       <c r="AL5" s="5"/>
       <c r="AM5" s="5"/>
-      <c r="AN5" s="65"/>
-      <c r="AO5" s="65"/>
-      <c r="AP5" s="65"/>
-      <c r="AQ5" s="65"/>
-      <c r="AR5" s="65"/>
-      <c r="AS5" s="65"/>
-      <c r="AT5" s="65"/>
-      <c r="AU5" s="65"/>
-      <c r="AV5" s="65"/>
+      <c r="AN5" s="64"/>
+      <c r="AO5" s="64"/>
+      <c r="AP5" s="64"/>
+      <c r="AQ5" s="64"/>
+      <c r="AR5" s="64"/>
+      <c r="AS5" s="64"/>
+      <c r="AT5" s="64"/>
+      <c r="AU5" s="64"/>
+      <c r="AV5" s="64"/>
     </row>
     <row r="6" spans="1:48">
       <c r="A6" s="2"/>
@@ -6418,15 +6297,15 @@
       <c r="AK6" s="6"/>
       <c r="AL6" s="6"/>
       <c r="AM6" s="6"/>
-      <c r="AN6" s="66"/>
-      <c r="AO6" s="66"/>
-      <c r="AP6" s="66"/>
-      <c r="AQ6" s="66"/>
-      <c r="AR6" s="66"/>
-      <c r="AS6" s="66"/>
-      <c r="AT6" s="66"/>
-      <c r="AU6" s="66"/>
-      <c r="AV6" s="66"/>
+      <c r="AN6" s="65"/>
+      <c r="AO6" s="65"/>
+      <c r="AP6" s="65"/>
+      <c r="AQ6" s="65"/>
+      <c r="AR6" s="65"/>
+      <c r="AS6" s="65"/>
+      <c r="AT6" s="65"/>
+      <c r="AU6" s="65"/>
+      <c r="AV6" s="65"/>
     </row>
     <row r="7" spans="1:48">
       <c r="A7" s="1"/>
@@ -6468,15 +6347,15 @@
       <c r="AK7" s="5"/>
       <c r="AL7" s="5"/>
       <c r="AM7" s="5"/>
-      <c r="AN7" s="65"/>
-      <c r="AO7" s="65"/>
-      <c r="AP7" s="65"/>
-      <c r="AQ7" s="65"/>
-      <c r="AR7" s="65"/>
-      <c r="AS7" s="65"/>
-      <c r="AT7" s="65"/>
-      <c r="AU7" s="65"/>
-      <c r="AV7" s="65"/>
+      <c r="AN7" s="64"/>
+      <c r="AO7" s="64"/>
+      <c r="AP7" s="64"/>
+      <c r="AQ7" s="64"/>
+      <c r="AR7" s="64"/>
+      <c r="AS7" s="64"/>
+      <c r="AT7" s="64"/>
+      <c r="AU7" s="64"/>
+      <c r="AV7" s="64"/>
     </row>
     <row r="8" spans="1:48">
       <c r="A8" s="2"/>
@@ -6518,15 +6397,15 @@
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
       <c r="AM8" s="6"/>
-      <c r="AN8" s="66"/>
-      <c r="AO8" s="66"/>
-      <c r="AP8" s="66"/>
-      <c r="AQ8" s="66"/>
-      <c r="AR8" s="66"/>
-      <c r="AS8" s="66"/>
-      <c r="AT8" s="66"/>
-      <c r="AU8" s="66"/>
-      <c r="AV8" s="66"/>
+      <c r="AN8" s="65"/>
+      <c r="AO8" s="65"/>
+      <c r="AP8" s="65"/>
+      <c r="AQ8" s="65"/>
+      <c r="AR8" s="65"/>
+      <c r="AS8" s="65"/>
+      <c r="AT8" s="65"/>
+      <c r="AU8" s="65"/>
+      <c r="AV8" s="65"/>
     </row>
     <row r="9" spans="1:48">
       <c r="A9" s="1"/>
@@ -6568,15 +6447,15 @@
       <c r="AK9" s="5"/>
       <c r="AL9" s="5"/>
       <c r="AM9" s="5"/>
-      <c r="AN9" s="65"/>
-      <c r="AO9" s="65"/>
-      <c r="AP9" s="65"/>
-      <c r="AQ9" s="65"/>
-      <c r="AR9" s="65"/>
-      <c r="AS9" s="65"/>
-      <c r="AT9" s="65"/>
-      <c r="AU9" s="65"/>
-      <c r="AV9" s="65"/>
+      <c r="AN9" s="64"/>
+      <c r="AO9" s="64"/>
+      <c r="AP9" s="64"/>
+      <c r="AQ9" s="64"/>
+      <c r="AR9" s="64"/>
+      <c r="AS9" s="64"/>
+      <c r="AT9" s="64"/>
+      <c r="AU9" s="64"/>
+      <c r="AV9" s="64"/>
     </row>
     <row r="10" spans="1:48">
       <c r="A10" s="2"/>
@@ -6618,15 +6497,15 @@
       <c r="AK10" s="6"/>
       <c r="AL10" s="6"/>
       <c r="AM10" s="6"/>
-      <c r="AN10" s="66"/>
-      <c r="AO10" s="66"/>
-      <c r="AP10" s="66"/>
-      <c r="AQ10" s="66"/>
-      <c r="AR10" s="66"/>
-      <c r="AS10" s="66"/>
-      <c r="AT10" s="66"/>
-      <c r="AU10" s="66"/>
-      <c r="AV10" s="66"/>
+      <c r="AN10" s="65"/>
+      <c r="AO10" s="65"/>
+      <c r="AP10" s="65"/>
+      <c r="AQ10" s="65"/>
+      <c r="AR10" s="65"/>
+      <c r="AS10" s="65"/>
+      <c r="AT10" s="65"/>
+      <c r="AU10" s="65"/>
+      <c r="AV10" s="65"/>
     </row>
     <row r="11" spans="1:48">
       <c r="A11" s="1"/>
@@ -6668,15 +6547,15 @@
       <c r="AK11" s="5"/>
       <c r="AL11" s="5"/>
       <c r="AM11" s="5"/>
-      <c r="AN11" s="65"/>
-      <c r="AO11" s="65"/>
-      <c r="AP11" s="65"/>
-      <c r="AQ11" s="65"/>
-      <c r="AR11" s="65"/>
-      <c r="AS11" s="65"/>
-      <c r="AT11" s="65"/>
-      <c r="AU11" s="65"/>
-      <c r="AV11" s="65"/>
+      <c r="AN11" s="64"/>
+      <c r="AO11" s="64"/>
+      <c r="AP11" s="64"/>
+      <c r="AQ11" s="64"/>
+      <c r="AR11" s="64"/>
+      <c r="AS11" s="64"/>
+      <c r="AT11" s="64"/>
+      <c r="AU11" s="64"/>
+      <c r="AV11" s="64"/>
     </row>
     <row r="12" spans="1:48">
       <c r="A12" s="2"/>
@@ -6718,15 +6597,15 @@
       <c r="AK12" s="6"/>
       <c r="AL12" s="6"/>
       <c r="AM12" s="6"/>
-      <c r="AN12" s="66"/>
-      <c r="AO12" s="66"/>
-      <c r="AP12" s="66"/>
-      <c r="AQ12" s="66"/>
-      <c r="AR12" s="66"/>
-      <c r="AS12" s="66"/>
-      <c r="AT12" s="66"/>
-      <c r="AU12" s="66"/>
-      <c r="AV12" s="66"/>
+      <c r="AN12" s="65"/>
+      <c r="AO12" s="65"/>
+      <c r="AP12" s="65"/>
+      <c r="AQ12" s="65"/>
+      <c r="AR12" s="65"/>
+      <c r="AS12" s="65"/>
+      <c r="AT12" s="65"/>
+      <c r="AU12" s="65"/>
+      <c r="AV12" s="65"/>
     </row>
     <row r="13" spans="1:48">
       <c r="A13" s="1"/>
@@ -6768,15 +6647,15 @@
       <c r="AK13" s="5"/>
       <c r="AL13" s="5"/>
       <c r="AM13" s="5"/>
-      <c r="AN13" s="65"/>
-      <c r="AO13" s="65"/>
-      <c r="AP13" s="65"/>
-      <c r="AQ13" s="65"/>
-      <c r="AR13" s="65"/>
-      <c r="AS13" s="65"/>
-      <c r="AT13" s="65"/>
-      <c r="AU13" s="65"/>
-      <c r="AV13" s="65"/>
+      <c r="AN13" s="64"/>
+      <c r="AO13" s="64"/>
+      <c r="AP13" s="64"/>
+      <c r="AQ13" s="64"/>
+      <c r="AR13" s="64"/>
+      <c r="AS13" s="64"/>
+      <c r="AT13" s="64"/>
+      <c r="AU13" s="64"/>
+      <c r="AV13" s="64"/>
     </row>
     <row r="14" spans="1:48">
       <c r="A14" s="2"/>
@@ -6818,15 +6697,15 @@
       <c r="AK14" s="6"/>
       <c r="AL14" s="6"/>
       <c r="AM14" s="6"/>
-      <c r="AN14" s="66"/>
-      <c r="AO14" s="66"/>
-      <c r="AP14" s="66"/>
-      <c r="AQ14" s="66"/>
-      <c r="AR14" s="66"/>
-      <c r="AS14" s="66"/>
-      <c r="AT14" s="66"/>
-      <c r="AU14" s="66"/>
-      <c r="AV14" s="66"/>
+      <c r="AN14" s="65"/>
+      <c r="AO14" s="65"/>
+      <c r="AP14" s="65"/>
+      <c r="AQ14" s="65"/>
+      <c r="AR14" s="65"/>
+      <c r="AS14" s="65"/>
+      <c r="AT14" s="65"/>
+      <c r="AU14" s="65"/>
+      <c r="AV14" s="65"/>
     </row>
     <row r="15" spans="1:48">
       <c r="A15" s="1"/>
@@ -6868,15 +6747,15 @@
       <c r="AK15" s="5"/>
       <c r="AL15" s="5"/>
       <c r="AM15" s="5"/>
-      <c r="AN15" s="65"/>
-      <c r="AO15" s="65"/>
-      <c r="AP15" s="65"/>
-      <c r="AQ15" s="65"/>
-      <c r="AR15" s="65"/>
-      <c r="AS15" s="65"/>
-      <c r="AT15" s="65"/>
-      <c r="AU15" s="65"/>
-      <c r="AV15" s="65"/>
+      <c r="AN15" s="64"/>
+      <c r="AO15" s="64"/>
+      <c r="AP15" s="64"/>
+      <c r="AQ15" s="64"/>
+      <c r="AR15" s="64"/>
+      <c r="AS15" s="64"/>
+      <c r="AT15" s="64"/>
+      <c r="AU15" s="64"/>
+      <c r="AV15" s="64"/>
     </row>
     <row r="16" spans="1:48">
       <c r="A16" s="2"/>
@@ -6918,15 +6797,15 @@
       <c r="AK16" s="6"/>
       <c r="AL16" s="6"/>
       <c r="AM16" s="6"/>
-      <c r="AN16" s="66"/>
-      <c r="AO16" s="66"/>
-      <c r="AP16" s="66"/>
-      <c r="AQ16" s="66"/>
-      <c r="AR16" s="66"/>
-      <c r="AS16" s="66"/>
-      <c r="AT16" s="66"/>
-      <c r="AU16" s="66"/>
-      <c r="AV16" s="66"/>
+      <c r="AN16" s="65"/>
+      <c r="AO16" s="65"/>
+      <c r="AP16" s="65"/>
+      <c r="AQ16" s="65"/>
+      <c r="AR16" s="65"/>
+      <c r="AS16" s="65"/>
+      <c r="AT16" s="65"/>
+      <c r="AU16" s="65"/>
+      <c r="AV16" s="65"/>
     </row>
     <row r="17" spans="1:48">
       <c r="A17" s="1"/>
@@ -6968,15 +6847,15 @@
       <c r="AK17" s="5"/>
       <c r="AL17" s="5"/>
       <c r="AM17" s="5"/>
-      <c r="AN17" s="65"/>
-      <c r="AO17" s="65"/>
-      <c r="AP17" s="65"/>
-      <c r="AQ17" s="65"/>
-      <c r="AR17" s="65"/>
-      <c r="AS17" s="65"/>
-      <c r="AT17" s="65"/>
-      <c r="AU17" s="65"/>
-      <c r="AV17" s="65"/>
+      <c r="AN17" s="64"/>
+      <c r="AO17" s="64"/>
+      <c r="AP17" s="64"/>
+      <c r="AQ17" s="64"/>
+      <c r="AR17" s="64"/>
+      <c r="AS17" s="64"/>
+      <c r="AT17" s="64"/>
+      <c r="AU17" s="64"/>
+      <c r="AV17" s="64"/>
     </row>
     <row r="18" spans="1:48">
       <c r="A18" s="2"/>
@@ -7018,15 +6897,15 @@
       <c r="AK18" s="6"/>
       <c r="AL18" s="6"/>
       <c r="AM18" s="6"/>
-      <c r="AN18" s="66"/>
-      <c r="AO18" s="66"/>
-      <c r="AP18" s="66"/>
-      <c r="AQ18" s="66"/>
-      <c r="AR18" s="66"/>
-      <c r="AS18" s="66"/>
-      <c r="AT18" s="66"/>
-      <c r="AU18" s="66"/>
-      <c r="AV18" s="66"/>
+      <c r="AN18" s="65"/>
+      <c r="AO18" s="65"/>
+      <c r="AP18" s="65"/>
+      <c r="AQ18" s="65"/>
+      <c r="AR18" s="65"/>
+      <c r="AS18" s="65"/>
+      <c r="AT18" s="65"/>
+      <c r="AU18" s="65"/>
+      <c r="AV18" s="65"/>
     </row>
     <row r="19" spans="1:48">
       <c r="A19" s="1"/>
@@ -7068,15 +6947,15 @@
       <c r="AK19" s="5"/>
       <c r="AL19" s="5"/>
       <c r="AM19" s="5"/>
-      <c r="AN19" s="65"/>
-      <c r="AO19" s="65"/>
-      <c r="AP19" s="65"/>
-      <c r="AQ19" s="65"/>
-      <c r="AR19" s="65"/>
-      <c r="AS19" s="65"/>
-      <c r="AT19" s="65"/>
-      <c r="AU19" s="65"/>
-      <c r="AV19" s="65"/>
+      <c r="AN19" s="64"/>
+      <c r="AO19" s="64"/>
+      <c r="AP19" s="64"/>
+      <c r="AQ19" s="64"/>
+      <c r="AR19" s="64"/>
+      <c r="AS19" s="64"/>
+      <c r="AT19" s="64"/>
+      <c r="AU19" s="64"/>
+      <c r="AV19" s="64"/>
     </row>
     <row r="20" spans="1:48">
       <c r="A20" s="2"/>
@@ -7118,15 +6997,15 @@
       <c r="AK20" s="6"/>
       <c r="AL20" s="6"/>
       <c r="AM20" s="6"/>
-      <c r="AN20" s="66"/>
-      <c r="AO20" s="66"/>
-      <c r="AP20" s="66"/>
-      <c r="AQ20" s="66"/>
-      <c r="AR20" s="66"/>
-      <c r="AS20" s="66"/>
-      <c r="AT20" s="66"/>
-      <c r="AU20" s="66"/>
-      <c r="AV20" s="66"/>
+      <c r="AN20" s="65"/>
+      <c r="AO20" s="65"/>
+      <c r="AP20" s="65"/>
+      <c r="AQ20" s="65"/>
+      <c r="AR20" s="65"/>
+      <c r="AS20" s="65"/>
+      <c r="AT20" s="65"/>
+      <c r="AU20" s="65"/>
+      <c r="AV20" s="65"/>
     </row>
     <row r="21" spans="1:48">
       <c r="A21" s="1"/>
@@ -7168,15 +7047,15 @@
       <c r="AK21" s="5"/>
       <c r="AL21" s="5"/>
       <c r="AM21" s="5"/>
-      <c r="AN21" s="65"/>
-      <c r="AO21" s="65"/>
-      <c r="AP21" s="65"/>
-      <c r="AQ21" s="65"/>
-      <c r="AR21" s="65"/>
-      <c r="AS21" s="65"/>
-      <c r="AT21" s="65"/>
-      <c r="AU21" s="65"/>
-      <c r="AV21" s="65"/>
+      <c r="AN21" s="64"/>
+      <c r="AO21" s="64"/>
+      <c r="AP21" s="64"/>
+      <c r="AQ21" s="64"/>
+      <c r="AR21" s="64"/>
+      <c r="AS21" s="64"/>
+      <c r="AT21" s="64"/>
+      <c r="AU21" s="64"/>
+      <c r="AV21" s="64"/>
     </row>
     <row r="22" spans="1:48">
       <c r="A22" s="2"/>
@@ -7218,15 +7097,15 @@
       <c r="AK22" s="6"/>
       <c r="AL22" s="6"/>
       <c r="AM22" s="6"/>
-      <c r="AN22" s="66"/>
-      <c r="AO22" s="66"/>
-      <c r="AP22" s="66"/>
-      <c r="AQ22" s="66"/>
-      <c r="AR22" s="66"/>
-      <c r="AS22" s="66"/>
-      <c r="AT22" s="66"/>
-      <c r="AU22" s="66"/>
-      <c r="AV22" s="66"/>
+      <c r="AN22" s="65"/>
+      <c r="AO22" s="65"/>
+      <c r="AP22" s="65"/>
+      <c r="AQ22" s="65"/>
+      <c r="AR22" s="65"/>
+      <c r="AS22" s="65"/>
+      <c r="AT22" s="65"/>
+      <c r="AU22" s="65"/>
+      <c r="AV22" s="65"/>
     </row>
     <row r="23" spans="1:48">
       <c r="A23" s="1"/>
@@ -7268,15 +7147,15 @@
       <c r="AK23" s="5"/>
       <c r="AL23" s="5"/>
       <c r="AM23" s="5"/>
-      <c r="AN23" s="65"/>
-      <c r="AO23" s="65"/>
-      <c r="AP23" s="65"/>
-      <c r="AQ23" s="65"/>
-      <c r="AR23" s="65"/>
-      <c r="AS23" s="65"/>
-      <c r="AT23" s="65"/>
-      <c r="AU23" s="65"/>
-      <c r="AV23" s="65"/>
+      <c r="AN23" s="64"/>
+      <c r="AO23" s="64"/>
+      <c r="AP23" s="64"/>
+      <c r="AQ23" s="64"/>
+      <c r="AR23" s="64"/>
+      <c r="AS23" s="64"/>
+      <c r="AT23" s="64"/>
+      <c r="AU23" s="64"/>
+      <c r="AV23" s="64"/>
     </row>
     <row r="24" spans="1:48">
       <c r="A24" s="2"/>
@@ -7318,15 +7197,15 @@
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
       <c r="AM24" s="6"/>
-      <c r="AN24" s="66"/>
-      <c r="AO24" s="66"/>
-      <c r="AP24" s="66"/>
-      <c r="AQ24" s="66"/>
-      <c r="AR24" s="66"/>
-      <c r="AS24" s="66"/>
-      <c r="AT24" s="66"/>
-      <c r="AU24" s="66"/>
-      <c r="AV24" s="66"/>
+      <c r="AN24" s="65"/>
+      <c r="AO24" s="65"/>
+      <c r="AP24" s="65"/>
+      <c r="AQ24" s="65"/>
+      <c r="AR24" s="65"/>
+      <c r="AS24" s="65"/>
+      <c r="AT24" s="65"/>
+      <c r="AU24" s="65"/>
+      <c r="AV24" s="65"/>
     </row>
     <row r="25" spans="1:48">
       <c r="A25" s="1"/>
@@ -7368,15 +7247,15 @@
       <c r="AK25" s="5"/>
       <c r="AL25" s="5"/>
       <c r="AM25" s="5"/>
-      <c r="AN25" s="65"/>
-      <c r="AO25" s="65"/>
-      <c r="AP25" s="65"/>
-      <c r="AQ25" s="65"/>
-      <c r="AR25" s="65"/>
-      <c r="AS25" s="65"/>
-      <c r="AT25" s="65"/>
-      <c r="AU25" s="65"/>
-      <c r="AV25" s="65"/>
+      <c r="AN25" s="64"/>
+      <c r="AO25" s="64"/>
+      <c r="AP25" s="64"/>
+      <c r="AQ25" s="64"/>
+      <c r="AR25" s="64"/>
+      <c r="AS25" s="64"/>
+      <c r="AT25" s="64"/>
+      <c r="AU25" s="64"/>
+      <c r="AV25" s="64"/>
     </row>
     <row r="26" spans="1:48">
       <c r="A26" s="2"/>
@@ -7418,15 +7297,15 @@
       <c r="AK26" s="6"/>
       <c r="AL26" s="6"/>
       <c r="AM26" s="6"/>
-      <c r="AN26" s="66"/>
-      <c r="AO26" s="66"/>
-      <c r="AP26" s="66"/>
-      <c r="AQ26" s="66"/>
-      <c r="AR26" s="66"/>
-      <c r="AS26" s="66"/>
-      <c r="AT26" s="66"/>
-      <c r="AU26" s="66"/>
-      <c r="AV26" s="66"/>
+      <c r="AN26" s="65"/>
+      <c r="AO26" s="65"/>
+      <c r="AP26" s="65"/>
+      <c r="AQ26" s="65"/>
+      <c r="AR26" s="65"/>
+      <c r="AS26" s="65"/>
+      <c r="AT26" s="65"/>
+      <c r="AU26" s="65"/>
+      <c r="AV26" s="65"/>
     </row>
     <row r="27" spans="1:48">
       <c r="A27" s="1"/>
@@ -7468,15 +7347,15 @@
       <c r="AK27" s="5"/>
       <c r="AL27" s="5"/>
       <c r="AM27" s="5"/>
-      <c r="AN27" s="65"/>
-      <c r="AO27" s="65"/>
-      <c r="AP27" s="65"/>
-      <c r="AQ27" s="65"/>
-      <c r="AR27" s="65"/>
-      <c r="AS27" s="65"/>
-      <c r="AT27" s="65"/>
-      <c r="AU27" s="65"/>
-      <c r="AV27" s="65"/>
+      <c r="AN27" s="64"/>
+      <c r="AO27" s="64"/>
+      <c r="AP27" s="64"/>
+      <c r="AQ27" s="64"/>
+      <c r="AR27" s="64"/>
+      <c r="AS27" s="64"/>
+      <c r="AT27" s="64"/>
+      <c r="AU27" s="64"/>
+      <c r="AV27" s="64"/>
     </row>
     <row r="28" spans="1:48">
       <c r="A28" s="2"/>
@@ -7518,15 +7397,15 @@
       <c r="AK28" s="6"/>
       <c r="AL28" s="6"/>
       <c r="AM28" s="6"/>
-      <c r="AN28" s="66"/>
-      <c r="AO28" s="66"/>
-      <c r="AP28" s="66"/>
-      <c r="AQ28" s="66"/>
-      <c r="AR28" s="66"/>
-      <c r="AS28" s="66"/>
-      <c r="AT28" s="66"/>
-      <c r="AU28" s="66"/>
-      <c r="AV28" s="66"/>
+      <c r="AN28" s="65"/>
+      <c r="AO28" s="65"/>
+      <c r="AP28" s="65"/>
+      <c r="AQ28" s="65"/>
+      <c r="AR28" s="65"/>
+      <c r="AS28" s="65"/>
+      <c r="AT28" s="65"/>
+      <c r="AU28" s="65"/>
+      <c r="AV28" s="65"/>
     </row>
     <row r="29" spans="1:48">
       <c r="A29" s="1"/>
@@ -7568,15 +7447,15 @@
       <c r="AK29" s="5"/>
       <c r="AL29" s="5"/>
       <c r="AM29" s="5"/>
-      <c r="AN29" s="65"/>
-      <c r="AO29" s="65"/>
-      <c r="AP29" s="65"/>
-      <c r="AQ29" s="65"/>
-      <c r="AR29" s="65"/>
-      <c r="AS29" s="65"/>
-      <c r="AT29" s="65"/>
-      <c r="AU29" s="65"/>
-      <c r="AV29" s="65"/>
+      <c r="AN29" s="64"/>
+      <c r="AO29" s="64"/>
+      <c r="AP29" s="64"/>
+      <c r="AQ29" s="64"/>
+      <c r="AR29" s="64"/>
+      <c r="AS29" s="64"/>
+      <c r="AT29" s="64"/>
+      <c r="AU29" s="64"/>
+      <c r="AV29" s="64"/>
     </row>
     <row r="30" spans="1:48">
       <c r="A30" s="2"/>
@@ -7618,15 +7497,15 @@
       <c r="AK30" s="6"/>
       <c r="AL30" s="6"/>
       <c r="AM30" s="6"/>
-      <c r="AN30" s="66"/>
-      <c r="AO30" s="66"/>
-      <c r="AP30" s="66"/>
-      <c r="AQ30" s="66"/>
-      <c r="AR30" s="66"/>
-      <c r="AS30" s="66"/>
-      <c r="AT30" s="66"/>
-      <c r="AU30" s="66"/>
-      <c r="AV30" s="66"/>
+      <c r="AN30" s="65"/>
+      <c r="AO30" s="65"/>
+      <c r="AP30" s="65"/>
+      <c r="AQ30" s="65"/>
+      <c r="AR30" s="65"/>
+      <c r="AS30" s="65"/>
+      <c r="AT30" s="65"/>
+      <c r="AU30" s="65"/>
+      <c r="AV30" s="65"/>
     </row>
     <row r="31" spans="1:48">
       <c r="A31" s="1"/>
@@ -7668,15 +7547,15 @@
       <c r="AK31" s="5"/>
       <c r="AL31" s="5"/>
       <c r="AM31" s="5"/>
-      <c r="AN31" s="65"/>
-      <c r="AO31" s="65"/>
-      <c r="AP31" s="65"/>
-      <c r="AQ31" s="65"/>
-      <c r="AR31" s="65"/>
-      <c r="AS31" s="65"/>
-      <c r="AT31" s="65"/>
-      <c r="AU31" s="65"/>
-      <c r="AV31" s="65"/>
+      <c r="AN31" s="64"/>
+      <c r="AO31" s="64"/>
+      <c r="AP31" s="64"/>
+      <c r="AQ31" s="64"/>
+      <c r="AR31" s="64"/>
+      <c r="AS31" s="64"/>
+      <c r="AT31" s="64"/>
+      <c r="AU31" s="64"/>
+      <c r="AV31" s="64"/>
     </row>
     <row r="32" spans="1:48">
       <c r="A32" s="2"/>
@@ -7718,15 +7597,15 @@
       <c r="AK32" s="6"/>
       <c r="AL32" s="6"/>
       <c r="AM32" s="6"/>
-      <c r="AN32" s="66"/>
-      <c r="AO32" s="66"/>
-      <c r="AP32" s="66"/>
-      <c r="AQ32" s="66"/>
-      <c r="AR32" s="66"/>
-      <c r="AS32" s="66"/>
-      <c r="AT32" s="66"/>
-      <c r="AU32" s="66"/>
-      <c r="AV32" s="66"/>
+      <c r="AN32" s="65"/>
+      <c r="AO32" s="65"/>
+      <c r="AP32" s="65"/>
+      <c r="AQ32" s="65"/>
+      <c r="AR32" s="65"/>
+      <c r="AS32" s="65"/>
+      <c r="AT32" s="65"/>
+      <c r="AU32" s="65"/>
+      <c r="AV32" s="65"/>
     </row>
     <row r="33" spans="1:48">
       <c r="A33" s="1"/>
@@ -7768,15 +7647,15 @@
       <c r="AK33" s="5"/>
       <c r="AL33" s="5"/>
       <c r="AM33" s="5"/>
-      <c r="AN33" s="65"/>
-      <c r="AO33" s="65"/>
-      <c r="AP33" s="65"/>
-      <c r="AQ33" s="65"/>
-      <c r="AR33" s="65"/>
-      <c r="AS33" s="65"/>
-      <c r="AT33" s="65"/>
-      <c r="AU33" s="65"/>
-      <c r="AV33" s="65"/>
+      <c r="AN33" s="64"/>
+      <c r="AO33" s="64"/>
+      <c r="AP33" s="64"/>
+      <c r="AQ33" s="64"/>
+      <c r="AR33" s="64"/>
+      <c r="AS33" s="64"/>
+      <c r="AT33" s="64"/>
+      <c r="AU33" s="64"/>
+      <c r="AV33" s="64"/>
     </row>
     <row r="34" spans="1:48">
       <c r="A34" s="2"/>
@@ -7818,15 +7697,15 @@
       <c r="AK34" s="6"/>
       <c r="AL34" s="6"/>
       <c r="AM34" s="6"/>
-      <c r="AN34" s="66"/>
-      <c r="AO34" s="66"/>
-      <c r="AP34" s="66"/>
-      <c r="AQ34" s="66"/>
-      <c r="AR34" s="66"/>
-      <c r="AS34" s="66"/>
-      <c r="AT34" s="66"/>
-      <c r="AU34" s="66"/>
-      <c r="AV34" s="66"/>
+      <c r="AN34" s="65"/>
+      <c r="AO34" s="65"/>
+      <c r="AP34" s="65"/>
+      <c r="AQ34" s="65"/>
+      <c r="AR34" s="65"/>
+      <c r="AS34" s="65"/>
+      <c r="AT34" s="65"/>
+      <c r="AU34" s="65"/>
+      <c r="AV34" s="65"/>
     </row>
     <row r="35" spans="1:48">
       <c r="A35" s="1"/>
@@ -7868,15 +7747,15 @@
       <c r="AK35" s="5"/>
       <c r="AL35" s="5"/>
       <c r="AM35" s="5"/>
-      <c r="AN35" s="65"/>
-      <c r="AO35" s="65"/>
-      <c r="AP35" s="65"/>
-      <c r="AQ35" s="65"/>
-      <c r="AR35" s="65"/>
-      <c r="AS35" s="65"/>
-      <c r="AT35" s="65"/>
-      <c r="AU35" s="65"/>
-      <c r="AV35" s="65"/>
+      <c r="AN35" s="64"/>
+      <c r="AO35" s="64"/>
+      <c r="AP35" s="64"/>
+      <c r="AQ35" s="64"/>
+      <c r="AR35" s="64"/>
+      <c r="AS35" s="64"/>
+      <c r="AT35" s="64"/>
+      <c r="AU35" s="64"/>
+      <c r="AV35" s="64"/>
     </row>
     <row r="36" spans="1:48">
       <c r="A36" s="2"/>
@@ -7918,15 +7797,15 @@
       <c r="AK36" s="6"/>
       <c r="AL36" s="6"/>
       <c r="AM36" s="6"/>
-      <c r="AN36" s="66"/>
-      <c r="AO36" s="66"/>
-      <c r="AP36" s="66"/>
-      <c r="AQ36" s="66"/>
-      <c r="AR36" s="66"/>
-      <c r="AS36" s="66"/>
-      <c r="AT36" s="66"/>
-      <c r="AU36" s="66"/>
-      <c r="AV36" s="66"/>
+      <c r="AN36" s="65"/>
+      <c r="AO36" s="65"/>
+      <c r="AP36" s="65"/>
+      <c r="AQ36" s="65"/>
+      <c r="AR36" s="65"/>
+      <c r="AS36" s="65"/>
+      <c r="AT36" s="65"/>
+      <c r="AU36" s="65"/>
+      <c r="AV36" s="65"/>
     </row>
     <row r="37" spans="1:48">
       <c r="A37" s="1"/>
@@ -7968,15 +7847,15 @@
       <c r="AK37" s="5"/>
       <c r="AL37" s="5"/>
       <c r="AM37" s="5"/>
-      <c r="AN37" s="65"/>
-      <c r="AO37" s="65"/>
-      <c r="AP37" s="65"/>
-      <c r="AQ37" s="65"/>
-      <c r="AR37" s="65"/>
-      <c r="AS37" s="65"/>
-      <c r="AT37" s="65"/>
-      <c r="AU37" s="65"/>
-      <c r="AV37" s="65"/>
+      <c r="AN37" s="64"/>
+      <c r="AO37" s="64"/>
+      <c r="AP37" s="64"/>
+      <c r="AQ37" s="64"/>
+      <c r="AR37" s="64"/>
+      <c r="AS37" s="64"/>
+      <c r="AT37" s="64"/>
+      <c r="AU37" s="64"/>
+      <c r="AV37" s="64"/>
     </row>
     <row r="38" spans="1:48">
       <c r="A38" s="2"/>
@@ -8018,15 +7897,15 @@
       <c r="AK38" s="6"/>
       <c r="AL38" s="6"/>
       <c r="AM38" s="6"/>
-      <c r="AN38" s="66"/>
-      <c r="AO38" s="66"/>
-      <c r="AP38" s="66"/>
-      <c r="AQ38" s="66"/>
-      <c r="AR38" s="66"/>
-      <c r="AS38" s="66"/>
-      <c r="AT38" s="66"/>
-      <c r="AU38" s="66"/>
-      <c r="AV38" s="66"/>
+      <c r="AN38" s="65"/>
+      <c r="AO38" s="65"/>
+      <c r="AP38" s="65"/>
+      <c r="AQ38" s="65"/>
+      <c r="AR38" s="65"/>
+      <c r="AS38" s="65"/>
+      <c r="AT38" s="65"/>
+      <c r="AU38" s="65"/>
+      <c r="AV38" s="65"/>
     </row>
     <row r="39" spans="1:48">
       <c r="A39" s="1"/>
@@ -8068,15 +7947,15 @@
       <c r="AK39" s="5"/>
       <c r="AL39" s="5"/>
       <c r="AM39" s="5"/>
-      <c r="AN39" s="65"/>
-      <c r="AO39" s="65"/>
-      <c r="AP39" s="65"/>
-      <c r="AQ39" s="65"/>
-      <c r="AR39" s="65"/>
-      <c r="AS39" s="65"/>
-      <c r="AT39" s="65"/>
-      <c r="AU39" s="65"/>
-      <c r="AV39" s="65"/>
+      <c r="AN39" s="64"/>
+      <c r="AO39" s="64"/>
+      <c r="AP39" s="64"/>
+      <c r="AQ39" s="64"/>
+      <c r="AR39" s="64"/>
+      <c r="AS39" s="64"/>
+      <c r="AT39" s="64"/>
+      <c r="AU39" s="64"/>
+      <c r="AV39" s="64"/>
     </row>
     <row r="40" spans="1:48">
       <c r="A40" s="2"/>
@@ -8118,15 +7997,15 @@
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
       <c r="AM40" s="6"/>
-      <c r="AN40" s="66"/>
-      <c r="AO40" s="66"/>
-      <c r="AP40" s="66"/>
-      <c r="AQ40" s="66"/>
-      <c r="AR40" s="66"/>
-      <c r="AS40" s="66"/>
-      <c r="AT40" s="66"/>
-      <c r="AU40" s="66"/>
-      <c r="AV40" s="66"/>
+      <c r="AN40" s="65"/>
+      <c r="AO40" s="65"/>
+      <c r="AP40" s="65"/>
+      <c r="AQ40" s="65"/>
+      <c r="AR40" s="65"/>
+      <c r="AS40" s="65"/>
+      <c r="AT40" s="65"/>
+      <c r="AU40" s="65"/>
+      <c r="AV40" s="65"/>
     </row>
     <row r="41" spans="1:48">
       <c r="A41" s="1"/>
@@ -8168,15 +8047,15 @@
       <c r="AK41" s="5"/>
       <c r="AL41" s="5"/>
       <c r="AM41" s="5"/>
-      <c r="AN41" s="65"/>
-      <c r="AO41" s="65"/>
-      <c r="AP41" s="65"/>
-      <c r="AQ41" s="65"/>
-      <c r="AR41" s="65"/>
-      <c r="AS41" s="65"/>
-      <c r="AT41" s="65"/>
-      <c r="AU41" s="65"/>
-      <c r="AV41" s="65"/>
+      <c r="AN41" s="64"/>
+      <c r="AO41" s="64"/>
+      <c r="AP41" s="64"/>
+      <c r="AQ41" s="64"/>
+      <c r="AR41" s="64"/>
+      <c r="AS41" s="64"/>
+      <c r="AT41" s="64"/>
+      <c r="AU41" s="64"/>
+      <c r="AV41" s="64"/>
     </row>
     <row r="42" spans="1:48">
       <c r="A42" s="2"/>
@@ -8218,15 +8097,15 @@
       <c r="AK42" s="6"/>
       <c r="AL42" s="6"/>
       <c r="AM42" s="6"/>
-      <c r="AN42" s="66"/>
-      <c r="AO42" s="66"/>
-      <c r="AP42" s="66"/>
-      <c r="AQ42" s="66"/>
-      <c r="AR42" s="66"/>
-      <c r="AS42" s="66"/>
-      <c r="AT42" s="66"/>
-      <c r="AU42" s="66"/>
-      <c r="AV42" s="66"/>
+      <c r="AN42" s="65"/>
+      <c r="AO42" s="65"/>
+      <c r="AP42" s="65"/>
+      <c r="AQ42" s="65"/>
+      <c r="AR42" s="65"/>
+      <c r="AS42" s="65"/>
+      <c r="AT42" s="65"/>
+      <c r="AU42" s="65"/>
+      <c r="AV42" s="65"/>
     </row>
     <row r="43" spans="1:48">
       <c r="A43" s="1"/>
@@ -8268,15 +8147,15 @@
       <c r="AK43" s="5"/>
       <c r="AL43" s="5"/>
       <c r="AM43" s="5"/>
-      <c r="AN43" s="65"/>
-      <c r="AO43" s="65"/>
-      <c r="AP43" s="65"/>
-      <c r="AQ43" s="65"/>
-      <c r="AR43" s="65"/>
-      <c r="AS43" s="65"/>
-      <c r="AT43" s="65"/>
-      <c r="AU43" s="65"/>
-      <c r="AV43" s="65"/>
+      <c r="AN43" s="64"/>
+      <c r="AO43" s="64"/>
+      <c r="AP43" s="64"/>
+      <c r="AQ43" s="64"/>
+      <c r="AR43" s="64"/>
+      <c r="AS43" s="64"/>
+      <c r="AT43" s="64"/>
+      <c r="AU43" s="64"/>
+      <c r="AV43" s="64"/>
     </row>
     <row r="44" spans="1:48">
       <c r="A44" s="2"/>
@@ -8318,15 +8197,15 @@
       <c r="AK44" s="6"/>
       <c r="AL44" s="6"/>
       <c r="AM44" s="6"/>
-      <c r="AN44" s="66"/>
-      <c r="AO44" s="66"/>
-      <c r="AP44" s="66"/>
-      <c r="AQ44" s="66"/>
-      <c r="AR44" s="66"/>
-      <c r="AS44" s="66"/>
-      <c r="AT44" s="66"/>
-      <c r="AU44" s="66"/>
-      <c r="AV44" s="66"/>
+      <c r="AN44" s="65"/>
+      <c r="AO44" s="65"/>
+      <c r="AP44" s="65"/>
+      <c r="AQ44" s="65"/>
+      <c r="AR44" s="65"/>
+      <c r="AS44" s="65"/>
+      <c r="AT44" s="65"/>
+      <c r="AU44" s="65"/>
+      <c r="AV44" s="65"/>
     </row>
     <row r="45" spans="1:48">
       <c r="A45" s="1"/>
@@ -8368,15 +8247,15 @@
       <c r="AK45" s="5"/>
       <c r="AL45" s="5"/>
       <c r="AM45" s="5"/>
-      <c r="AN45" s="65"/>
-      <c r="AO45" s="65"/>
-      <c r="AP45" s="65"/>
-      <c r="AQ45" s="65"/>
-      <c r="AR45" s="65"/>
-      <c r="AS45" s="65"/>
-      <c r="AT45" s="65"/>
-      <c r="AU45" s="65"/>
-      <c r="AV45" s="65"/>
+      <c r="AN45" s="64"/>
+      <c r="AO45" s="64"/>
+      <c r="AP45" s="64"/>
+      <c r="AQ45" s="64"/>
+      <c r="AR45" s="64"/>
+      <c r="AS45" s="64"/>
+      <c r="AT45" s="64"/>
+      <c r="AU45" s="64"/>
+      <c r="AV45" s="64"/>
     </row>
     <row r="46" spans="1:48">
       <c r="A46" s="2"/>
@@ -8418,15 +8297,15 @@
       <c r="AK46" s="6"/>
       <c r="AL46" s="6"/>
       <c r="AM46" s="6"/>
-      <c r="AN46" s="66"/>
-      <c r="AO46" s="66"/>
-      <c r="AP46" s="66"/>
-      <c r="AQ46" s="66"/>
-      <c r="AR46" s="66"/>
-      <c r="AS46" s="66"/>
-      <c r="AT46" s="66"/>
-      <c r="AU46" s="66"/>
-      <c r="AV46" s="66"/>
+      <c r="AN46" s="65"/>
+      <c r="AO46" s="65"/>
+      <c r="AP46" s="65"/>
+      <c r="AQ46" s="65"/>
+      <c r="AR46" s="65"/>
+      <c r="AS46" s="65"/>
+      <c r="AT46" s="65"/>
+      <c r="AU46" s="65"/>
+      <c r="AV46" s="65"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C8">
@@ -8498,10 +8377,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="H1" s="36" t="s">
         <v>8</v>
@@ -8524,17 +8403,17 @@
       <c r="N1" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="67" t="s">
+      <c r="O1" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="68" t="s">
-        <v>111</v>
+      <c r="P1" s="67" t="s">
+        <v>93</v>
       </c>
       <c r="Q1" s="36" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="R1" s="36" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="S1" s="36" t="s">
         <v>12</v>
@@ -8542,88 +8421,88 @@
       <c r="T1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="67" t="s">
+      <c r="U1" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="68" t="s">
-        <v>80</v>
+      <c r="V1" s="67" t="s">
+        <v>62</v>
       </c>
       <c r="W1" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" s="66" t="s">
         <v>47</v>
       </c>
       <c r="Y1" s="37" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="Z1" s="46" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="AA1" s="46" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="AB1" s="46" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="AC1" s="46" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="11" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="M2" s="47" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="N2" s="47" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="O2" s="51" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="P2" s="49" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="Q2" s="50" t="s">
         <v>48</v>
       </c>
       <c r="R2" s="50" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="S2" s="50" t="s">
         <v>29</v>
@@ -8631,8 +8510,8 @@
       <c r="T2" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="U2" s="69" t="s">
-        <v>101</v>
+      <c r="U2" s="68" t="s">
+        <v>83</v>
       </c>
       <c r="V2" s="49" t="s">
         <v>29</v>
@@ -8640,23 +8519,23 @@
       <c r="W2" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="X2" s="69" t="s">
-        <v>101</v>
+      <c r="X2" s="68" t="s">
+        <v>83</v>
       </c>
       <c r="Y2" s="15" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="Z2" s="53" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="AA2" s="53" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="AB2" s="53" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="AC2" s="53" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:29">
@@ -8685,10 +8564,10 @@
       <c r="W3" s="1"/>
       <c r="X3" s="20"/>
       <c r="Y3" s="7"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="70"/>
-      <c r="AC3" s="70"/>
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="69"/>
+      <c r="AB3" s="69"/>
+      <c r="AC3" s="69"/>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="2"/>
@@ -8716,10 +8595,10 @@
       <c r="W4" s="2"/>
       <c r="X4" s="18"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="71"/>
-      <c r="AA4" s="71"/>
-      <c r="AB4" s="71"/>
-      <c r="AC4" s="71"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
+      <c r="AC4" s="70"/>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="1"/>
@@ -8747,10 +8626,10 @@
       <c r="W5" s="1"/>
       <c r="X5" s="20"/>
       <c r="Y5" s="7"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="70"/>
-      <c r="AB5" s="70"/>
-      <c r="AC5" s="70"/>
+      <c r="Z5" s="69"/>
+      <c r="AA5" s="69"/>
+      <c r="AB5" s="69"/>
+      <c r="AC5" s="69"/>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="2"/>
@@ -8778,10 +8657,10 @@
       <c r="W6" s="2"/>
       <c r="X6" s="18"/>
       <c r="Y6" s="8"/>
-      <c r="Z6" s="71"/>
-      <c r="AA6" s="71"/>
-      <c r="AB6" s="71"/>
-      <c r="AC6" s="71"/>
+      <c r="Z6" s="70"/>
+      <c r="AA6" s="70"/>
+      <c r="AB6" s="70"/>
+      <c r="AC6" s="70"/>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="1"/>
@@ -8809,10 +8688,10 @@
       <c r="W7" s="1"/>
       <c r="X7" s="20"/>
       <c r="Y7" s="7"/>
-      <c r="Z7" s="70"/>
-      <c r="AA7" s="70"/>
-      <c r="AB7" s="70"/>
-      <c r="AC7" s="70"/>
+      <c r="Z7" s="69"/>
+      <c r="AA7" s="69"/>
+      <c r="AB7" s="69"/>
+      <c r="AC7" s="69"/>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="2"/>
@@ -8840,10 +8719,10 @@
       <c r="W8" s="2"/>
       <c r="X8" s="18"/>
       <c r="Y8" s="8"/>
-      <c r="Z8" s="71"/>
-      <c r="AA8" s="71"/>
-      <c r="AB8" s="71"/>
-      <c r="AC8" s="71"/>
+      <c r="Z8" s="70"/>
+      <c r="AA8" s="70"/>
+      <c r="AB8" s="70"/>
+      <c r="AC8" s="70"/>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="1"/>
@@ -8871,10 +8750,10 @@
       <c r="W9" s="1"/>
       <c r="X9" s="20"/>
       <c r="Y9" s="7"/>
-      <c r="Z9" s="70"/>
-      <c r="AA9" s="70"/>
-      <c r="AB9" s="70"/>
-      <c r="AC9" s="70"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="69"/>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="2"/>
@@ -8902,10 +8781,10 @@
       <c r="W10" s="2"/>
       <c r="X10" s="18"/>
       <c r="Y10" s="8"/>
-      <c r="Z10" s="71"/>
-      <c r="AA10" s="71"/>
-      <c r="AB10" s="71"/>
-      <c r="AC10" s="71"/>
+      <c r="Z10" s="70"/>
+      <c r="AA10" s="70"/>
+      <c r="AB10" s="70"/>
+      <c r="AC10" s="70"/>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="1"/>
@@ -8933,10 +8812,10 @@
       <c r="W11" s="1"/>
       <c r="X11" s="20"/>
       <c r="Y11" s="7"/>
-      <c r="Z11" s="70"/>
-      <c r="AA11" s="70"/>
-      <c r="AB11" s="70"/>
-      <c r="AC11" s="70"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="69"/>
+      <c r="AC11" s="69"/>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="2"/>
@@ -8964,10 +8843,10 @@
       <c r="W12" s="2"/>
       <c r="X12" s="18"/>
       <c r="Y12" s="8"/>
-      <c r="Z12" s="71"/>
-      <c r="AA12" s="71"/>
-      <c r="AB12" s="71"/>
-      <c r="AC12" s="71"/>
+      <c r="Z12" s="70"/>
+      <c r="AA12" s="70"/>
+      <c r="AB12" s="70"/>
+      <c r="AC12" s="70"/>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="1"/>
@@ -8995,10 +8874,10 @@
       <c r="W13" s="1"/>
       <c r="X13" s="20"/>
       <c r="Y13" s="7"/>
-      <c r="Z13" s="70"/>
-      <c r="AA13" s="70"/>
-      <c r="AB13" s="70"/>
-      <c r="AC13" s="70"/>
+      <c r="Z13" s="69"/>
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="69"/>
+      <c r="AC13" s="69"/>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="2"/>
@@ -9026,10 +8905,10 @@
       <c r="W14" s="2"/>
       <c r="X14" s="18"/>
       <c r="Y14" s="8"/>
-      <c r="Z14" s="71"/>
-      <c r="AA14" s="71"/>
-      <c r="AB14" s="71"/>
-      <c r="AC14" s="71"/>
+      <c r="Z14" s="70"/>
+      <c r="AA14" s="70"/>
+      <c r="AB14" s="70"/>
+      <c r="AC14" s="70"/>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="1"/>
@@ -9057,10 +8936,10 @@
       <c r="W15" s="1"/>
       <c r="X15" s="20"/>
       <c r="Y15" s="7"/>
-      <c r="Z15" s="70"/>
-      <c r="AA15" s="70"/>
-      <c r="AB15" s="70"/>
-      <c r="AC15" s="70"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="69"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="2"/>
@@ -9088,10 +8967,10 @@
       <c r="W16" s="2"/>
       <c r="X16" s="18"/>
       <c r="Y16" s="8"/>
-      <c r="Z16" s="71"/>
-      <c r="AA16" s="71"/>
-      <c r="AB16" s="71"/>
-      <c r="AC16" s="71"/>
+      <c r="Z16" s="70"/>
+      <c r="AA16" s="70"/>
+      <c r="AB16" s="70"/>
+      <c r="AC16" s="70"/>
     </row>
     <row r="17" spans="1:29">
       <c r="A17" s="1"/>
@@ -9119,10 +8998,10 @@
       <c r="W17" s="1"/>
       <c r="X17" s="20"/>
       <c r="Y17" s="7"/>
-      <c r="Z17" s="70"/>
-      <c r="AA17" s="70"/>
-      <c r="AB17" s="70"/>
-      <c r="AC17" s="70"/>
+      <c r="Z17" s="69"/>
+      <c r="AA17" s="69"/>
+      <c r="AB17" s="69"/>
+      <c r="AC17" s="69"/>
     </row>
     <row r="18" spans="1:29">
       <c r="A18" s="2"/>
@@ -9150,10 +9029,10 @@
       <c r="W18" s="2"/>
       <c r="X18" s="18"/>
       <c r="Y18" s="8"/>
-      <c r="Z18" s="71"/>
-      <c r="AA18" s="71"/>
-      <c r="AB18" s="71"/>
-      <c r="AC18" s="71"/>
+      <c r="Z18" s="70"/>
+      <c r="AA18" s="70"/>
+      <c r="AB18" s="70"/>
+      <c r="AC18" s="70"/>
     </row>
     <row r="19" spans="1:29">
       <c r="A19" s="1"/>
@@ -9181,10 +9060,10 @@
       <c r="W19" s="1"/>
       <c r="X19" s="20"/>
       <c r="Y19" s="7"/>
-      <c r="Z19" s="70"/>
-      <c r="AA19" s="70"/>
-      <c r="AB19" s="70"/>
-      <c r="AC19" s="70"/>
+      <c r="Z19" s="69"/>
+      <c r="AA19" s="69"/>
+      <c r="AB19" s="69"/>
+      <c r="AC19" s="69"/>
     </row>
     <row r="20" spans="1:29">
       <c r="A20" s="2"/>
@@ -9212,10 +9091,10 @@
       <c r="W20" s="2"/>
       <c r="X20" s="18"/>
       <c r="Y20" s="8"/>
-      <c r="Z20" s="71"/>
-      <c r="AA20" s="71"/>
-      <c r="AB20" s="71"/>
-      <c r="AC20" s="71"/>
+      <c r="Z20" s="70"/>
+      <c r="AA20" s="70"/>
+      <c r="AB20" s="70"/>
+      <c r="AC20" s="70"/>
     </row>
     <row r="21" spans="1:29">
       <c r="A21" s="1"/>
@@ -9243,10 +9122,10 @@
       <c r="W21" s="1"/>
       <c r="X21" s="20"/>
       <c r="Y21" s="7"/>
-      <c r="Z21" s="70"/>
-      <c r="AA21" s="70"/>
-      <c r="AB21" s="70"/>
-      <c r="AC21" s="70"/>
+      <c r="Z21" s="69"/>
+      <c r="AA21" s="69"/>
+      <c r="AB21" s="69"/>
+      <c r="AC21" s="69"/>
     </row>
     <row r="22" spans="1:29">
       <c r="A22" s="2"/>
@@ -9274,10 +9153,10 @@
       <c r="W22" s="2"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="8"/>
-      <c r="Z22" s="71"/>
-      <c r="AA22" s="71"/>
-      <c r="AB22" s="71"/>
-      <c r="AC22" s="71"/>
+      <c r="Z22" s="70"/>
+      <c r="AA22" s="70"/>
+      <c r="AB22" s="70"/>
+      <c r="AC22" s="70"/>
     </row>
     <row r="23" spans="1:29">
       <c r="A23" s="1"/>
@@ -9305,10 +9184,10 @@
       <c r="W23" s="1"/>
       <c r="X23" s="20"/>
       <c r="Y23" s="7"/>
-      <c r="Z23" s="70"/>
-      <c r="AA23" s="70"/>
-      <c r="AB23" s="70"/>
-      <c r="AC23" s="70"/>
+      <c r="Z23" s="69"/>
+      <c r="AA23" s="69"/>
+      <c r="AB23" s="69"/>
+      <c r="AC23" s="69"/>
     </row>
     <row r="24" spans="1:29">
       <c r="A24" s="2"/>
@@ -9336,10 +9215,10 @@
       <c r="W24" s="2"/>
       <c r="X24" s="18"/>
       <c r="Y24" s="8"/>
-      <c r="Z24" s="71"/>
-      <c r="AA24" s="71"/>
-      <c r="AB24" s="71"/>
-      <c r="AC24" s="71"/>
+      <c r="Z24" s="70"/>
+      <c r="AA24" s="70"/>
+      <c r="AB24" s="70"/>
+      <c r="AC24" s="70"/>
     </row>
     <row r="25" spans="1:29">
       <c r="A25" s="1"/>
@@ -9367,10 +9246,10 @@
       <c r="W25" s="1"/>
       <c r="X25" s="20"/>
       <c r="Y25" s="7"/>
-      <c r="Z25" s="70"/>
-      <c r="AA25" s="70"/>
-      <c r="AB25" s="70"/>
-      <c r="AC25" s="70"/>
+      <c r="Z25" s="69"/>
+      <c r="AA25" s="69"/>
+      <c r="AB25" s="69"/>
+      <c r="AC25" s="69"/>
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="2"/>
@@ -9398,10 +9277,10 @@
       <c r="W26" s="2"/>
       <c r="X26" s="18"/>
       <c r="Y26" s="8"/>
-      <c r="Z26" s="71"/>
-      <c r="AA26" s="71"/>
-      <c r="AB26" s="71"/>
-      <c r="AC26" s="71"/>
+      <c r="Z26" s="70"/>
+      <c r="AA26" s="70"/>
+      <c r="AB26" s="70"/>
+      <c r="AC26" s="70"/>
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="1"/>
@@ -9429,10 +9308,10 @@
       <c r="W27" s="1"/>
       <c r="X27" s="20"/>
       <c r="Y27" s="7"/>
-      <c r="Z27" s="70"/>
-      <c r="AA27" s="70"/>
-      <c r="AB27" s="70"/>
-      <c r="AC27" s="70"/>
+      <c r="Z27" s="69"/>
+      <c r="AA27" s="69"/>
+      <c r="AB27" s="69"/>
+      <c r="AC27" s="69"/>
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="2"/>
@@ -9460,10 +9339,10 @@
       <c r="W28" s="2"/>
       <c r="X28" s="18"/>
       <c r="Y28" s="8"/>
-      <c r="Z28" s="71"/>
-      <c r="AA28" s="71"/>
-      <c r="AB28" s="71"/>
-      <c r="AC28" s="71"/>
+      <c r="Z28" s="70"/>
+      <c r="AA28" s="70"/>
+      <c r="AB28" s="70"/>
+      <c r="AC28" s="70"/>
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="1"/>
@@ -9491,10 +9370,10 @@
       <c r="W29" s="1"/>
       <c r="X29" s="20"/>
       <c r="Y29" s="7"/>
-      <c r="Z29" s="70"/>
-      <c r="AA29" s="70"/>
-      <c r="AB29" s="70"/>
-      <c r="AC29" s="70"/>
+      <c r="Z29" s="69"/>
+      <c r="AA29" s="69"/>
+      <c r="AB29" s="69"/>
+      <c r="AC29" s="69"/>
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="2"/>
@@ -9522,10 +9401,10 @@
       <c r="W30" s="2"/>
       <c r="X30" s="18"/>
       <c r="Y30" s="8"/>
-      <c r="Z30" s="71"/>
-      <c r="AA30" s="71"/>
-      <c r="AB30" s="71"/>
-      <c r="AC30" s="71"/>
+      <c r="Z30" s="70"/>
+      <c r="AA30" s="70"/>
+      <c r="AB30" s="70"/>
+      <c r="AC30" s="70"/>
     </row>
     <row r="31" spans="1:29">
       <c r="A31" s="1"/>
@@ -9553,10 +9432,10 @@
       <c r="W31" s="1"/>
       <c r="X31" s="20"/>
       <c r="Y31" s="7"/>
-      <c r="Z31" s="70"/>
-      <c r="AA31" s="70"/>
-      <c r="AB31" s="70"/>
-      <c r="AC31" s="70"/>
+      <c r="Z31" s="69"/>
+      <c r="AA31" s="69"/>
+      <c r="AB31" s="69"/>
+      <c r="AC31" s="69"/>
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="2"/>
@@ -9584,10 +9463,10 @@
       <c r="W32" s="2"/>
       <c r="X32" s="18"/>
       <c r="Y32" s="8"/>
-      <c r="Z32" s="71"/>
-      <c r="AA32" s="71"/>
-      <c r="AB32" s="71"/>
-      <c r="AC32" s="71"/>
+      <c r="Z32" s="70"/>
+      <c r="AA32" s="70"/>
+      <c r="AB32" s="70"/>
+      <c r="AC32" s="70"/>
     </row>
     <row r="33" spans="1:29">
       <c r="A33" s="1"/>
@@ -9615,10 +9494,10 @@
       <c r="W33" s="1"/>
       <c r="X33" s="20"/>
       <c r="Y33" s="7"/>
-      <c r="Z33" s="70"/>
-      <c r="AA33" s="70"/>
-      <c r="AB33" s="70"/>
-      <c r="AC33" s="70"/>
+      <c r="Z33" s="69"/>
+      <c r="AA33" s="69"/>
+      <c r="AB33" s="69"/>
+      <c r="AC33" s="69"/>
     </row>
     <row r="34" spans="1:29">
       <c r="A34" s="2"/>
@@ -9646,10 +9525,10 @@
       <c r="W34" s="2"/>
       <c r="X34" s="18"/>
       <c r="Y34" s="8"/>
-      <c r="Z34" s="71"/>
-      <c r="AA34" s="71"/>
-      <c r="AB34" s="71"/>
-      <c r="AC34" s="71"/>
+      <c r="Z34" s="70"/>
+      <c r="AA34" s="70"/>
+      <c r="AB34" s="70"/>
+      <c r="AC34" s="70"/>
     </row>
     <row r="35" spans="1:29">
       <c r="A35" s="1"/>
@@ -9677,10 +9556,10 @@
       <c r="W35" s="1"/>
       <c r="X35" s="20"/>
       <c r="Y35" s="7"/>
-      <c r="Z35" s="70"/>
-      <c r="AA35" s="70"/>
-      <c r="AB35" s="70"/>
-      <c r="AC35" s="70"/>
+      <c r="Z35" s="69"/>
+      <c r="AA35" s="69"/>
+      <c r="AB35" s="69"/>
+      <c r="AC35" s="69"/>
     </row>
     <row r="36" spans="1:29">
       <c r="A36" s="2"/>
@@ -9708,10 +9587,10 @@
       <c r="W36" s="2"/>
       <c r="X36" s="18"/>
       <c r="Y36" s="8"/>
-      <c r="Z36" s="71"/>
-      <c r="AA36" s="71"/>
-      <c r="AB36" s="71"/>
-      <c r="AC36" s="71"/>
+      <c r="Z36" s="70"/>
+      <c r="AA36" s="70"/>
+      <c r="AB36" s="70"/>
+      <c r="AC36" s="70"/>
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="1"/>
@@ -9739,10 +9618,10 @@
       <c r="W37" s="1"/>
       <c r="X37" s="20"/>
       <c r="Y37" s="7"/>
-      <c r="Z37" s="70"/>
-      <c r="AA37" s="70"/>
-      <c r="AB37" s="70"/>
-      <c r="AC37" s="70"/>
+      <c r="Z37" s="69"/>
+      <c r="AA37" s="69"/>
+      <c r="AB37" s="69"/>
+      <c r="AC37" s="69"/>
     </row>
     <row r="38" spans="1:29">
       <c r="A38" s="2"/>
@@ -9770,10 +9649,10 @@
       <c r="W38" s="2"/>
       <c r="X38" s="18"/>
       <c r="Y38" s="8"/>
-      <c r="Z38" s="71"/>
-      <c r="AA38" s="71"/>
-      <c r="AB38" s="71"/>
-      <c r="AC38" s="71"/>
+      <c r="Z38" s="70"/>
+      <c r="AA38" s="70"/>
+      <c r="AB38" s="70"/>
+      <c r="AC38" s="70"/>
     </row>
     <row r="39" spans="1:29">
       <c r="A39" s="1"/>
@@ -9801,10 +9680,10 @@
       <c r="W39" s="1"/>
       <c r="X39" s="20"/>
       <c r="Y39" s="7"/>
-      <c r="Z39" s="70"/>
-      <c r="AA39" s="70"/>
-      <c r="AB39" s="70"/>
-      <c r="AC39" s="70"/>
+      <c r="Z39" s="69"/>
+      <c r="AA39" s="69"/>
+      <c r="AB39" s="69"/>
+      <c r="AC39" s="69"/>
     </row>
     <row r="40" spans="1:29">
       <c r="A40" s="2"/>
@@ -9832,10 +9711,10 @@
       <c r="W40" s="2"/>
       <c r="X40" s="18"/>
       <c r="Y40" s="8"/>
-      <c r="Z40" s="71"/>
-      <c r="AA40" s="71"/>
-      <c r="AB40" s="71"/>
-      <c r="AC40" s="71"/>
+      <c r="Z40" s="70"/>
+      <c r="AA40" s="70"/>
+      <c r="AB40" s="70"/>
+      <c r="AC40" s="70"/>
     </row>
     <row r="41" spans="1:29">
       <c r="A41" s="1"/>
@@ -9863,10 +9742,10 @@
       <c r="W41" s="1"/>
       <c r="X41" s="20"/>
       <c r="Y41" s="7"/>
-      <c r="Z41" s="70"/>
-      <c r="AA41" s="70"/>
-      <c r="AB41" s="70"/>
-      <c r="AC41" s="70"/>
+      <c r="Z41" s="69"/>
+      <c r="AA41" s="69"/>
+      <c r="AB41" s="69"/>
+      <c r="AC41" s="69"/>
     </row>
     <row r="42" spans="1:29">
       <c r="A42" s="2"/>
@@ -9894,10 +9773,10 @@
       <c r="W42" s="2"/>
       <c r="X42" s="18"/>
       <c r="Y42" s="8"/>
-      <c r="Z42" s="71"/>
-      <c r="AA42" s="71"/>
-      <c r="AB42" s="71"/>
-      <c r="AC42" s="71"/>
+      <c r="Z42" s="70"/>
+      <c r="AA42" s="70"/>
+      <c r="AB42" s="70"/>
+      <c r="AC42" s="70"/>
     </row>
     <row r="43" spans="1:29">
       <c r="A43" s="1"/>
@@ -9925,10 +9804,10 @@
       <c r="W43" s="1"/>
       <c r="X43" s="20"/>
       <c r="Y43" s="7"/>
-      <c r="Z43" s="70"/>
-      <c r="AA43" s="70"/>
-      <c r="AB43" s="70"/>
-      <c r="AC43" s="70"/>
+      <c r="Z43" s="69"/>
+      <c r="AA43" s="69"/>
+      <c r="AB43" s="69"/>
+      <c r="AC43" s="69"/>
     </row>
     <row r="44" spans="1:29">
       <c r="A44" s="2"/>
@@ -9956,10 +9835,10 @@
       <c r="W44" s="2"/>
       <c r="X44" s="18"/>
       <c r="Y44" s="8"/>
-      <c r="Z44" s="71"/>
-      <c r="AA44" s="71"/>
-      <c r="AB44" s="71"/>
-      <c r="AC44" s="71"/>
+      <c r="Z44" s="70"/>
+      <c r="AA44" s="70"/>
+      <c r="AB44" s="70"/>
+      <c r="AC44" s="70"/>
     </row>
     <row r="45" spans="1:29">
       <c r="A45" s="1"/>
@@ -9987,10 +9866,10 @@
       <c r="W45" s="1"/>
       <c r="X45" s="20"/>
       <c r="Y45" s="7"/>
-      <c r="Z45" s="70"/>
-      <c r="AA45" s="70"/>
-      <c r="AB45" s="70"/>
-      <c r="AC45" s="70"/>
+      <c r="Z45" s="69"/>
+      <c r="AA45" s="69"/>
+      <c r="AB45" s="69"/>
+      <c r="AC45" s="69"/>
     </row>
     <row r="46" spans="1:29">
       <c r="A46" s="2"/>
@@ -10018,10 +9897,10 @@
       <c r="W46" s="2"/>
       <c r="X46" s="18"/>
       <c r="Y46" s="8"/>
-      <c r="Z46" s="71"/>
-      <c r="AA46" s="71"/>
-      <c r="AB46" s="71"/>
-      <c r="AC46" s="71"/>
+      <c r="Z46" s="70"/>
+      <c r="AA46" s="70"/>
+      <c r="AB46" s="70"/>
+      <c r="AC46" s="70"/>
     </row>
     <row r="47" spans="1:29">
       <c r="A47" s="1"/>
@@ -10049,10 +9928,10 @@
       <c r="W47" s="1"/>
       <c r="X47" s="20"/>
       <c r="Y47" s="7"/>
-      <c r="Z47" s="70"/>
-      <c r="AA47" s="70"/>
-      <c r="AB47" s="70"/>
-      <c r="AC47" s="70"/>
+      <c r="Z47" s="69"/>
+      <c r="AA47" s="69"/>
+      <c r="AB47" s="69"/>
+      <c r="AC47" s="69"/>
     </row>
     <row r="48" spans="1:29">
       <c r="A48" s="2"/>
@@ -10080,10 +9959,10 @@
       <c r="W48" s="2"/>
       <c r="X48" s="18"/>
       <c r="Y48" s="8"/>
-      <c r="Z48" s="71"/>
-      <c r="AA48" s="71"/>
-      <c r="AB48" s="71"/>
-      <c r="AC48" s="71"/>
+      <c r="Z48" s="70"/>
+      <c r="AA48" s="70"/>
+      <c r="AB48" s="70"/>
+      <c r="AC48" s="70"/>
     </row>
     <row r="49" spans="1:29">
       <c r="A49" s="1"/>
@@ -10111,10 +9990,10 @@
       <c r="W49" s="1"/>
       <c r="X49" s="20"/>
       <c r="Y49" s="7"/>
-      <c r="Z49" s="70"/>
-      <c r="AA49" s="70"/>
-      <c r="AB49" s="70"/>
-      <c r="AC49" s="70"/>
+      <c r="Z49" s="69"/>
+      <c r="AA49" s="69"/>
+      <c r="AB49" s="69"/>
+      <c r="AC49" s="69"/>
     </row>
     <row r="50" spans="1:29">
       <c r="A50" s="2"/>
@@ -10142,10 +10021,10 @@
       <c r="W50" s="2"/>
       <c r="X50" s="18"/>
       <c r="Y50" s="8"/>
-      <c r="Z50" s="71"/>
-      <c r="AA50" s="71"/>
-      <c r="AB50" s="71"/>
-      <c r="AC50" s="71"/>
+      <c r="Z50" s="70"/>
+      <c r="AA50" s="70"/>
+      <c r="AB50" s="70"/>
+      <c r="AC50" s="70"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -10197,10 +10076,10 @@
         <v>18</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="G1" s="36" t="s">
         <v>3</v>
@@ -10215,13 +10094,13 @@
         <v>46</v>
       </c>
       <c r="K1" s="43" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="L1" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="M1" s="73" t="s">
-        <v>153</v>
+        <v>94</v>
+      </c>
+      <c r="M1" s="72" t="s">
+        <v>135</v>
       </c>
       <c r="N1" s="43" t="s">
         <v>13</v>
@@ -10230,7 +10109,7 @@
         <v>43</v>
       </c>
       <c r="P1" s="43" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="Q1" s="43" t="s">
         <v>47</v>
@@ -10238,25 +10117,25 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="11" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="H2" s="47" t="s">
         <v>34</v>
@@ -10268,13 +10147,13 @@
         <v>34</v>
       </c>
       <c r="K2" s="50" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="L2" s="50" t="s">
         <v>48</v>
       </c>
       <c r="M2" s="50" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="N2" s="50" t="s">
         <v>29</v>
@@ -11227,22 +11106,22 @@
         <v>11</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="J1" s="35" t="s">
         <v>43</v>
@@ -11253,37 +11132,37 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="11" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>